<commit_message>
多系统 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/doc/接口协议.xlsx
+++ b/doc/接口协议.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17870"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="825" windowWidth="14805" windowHeight="7290"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="392">
   <si>
     <t>请求url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1531,14 +1531,22 @@
   </si>
   <si>
     <t>应用名称，每页的条数，第几页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册组织</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mulorgan!registOrgan</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2016,7 +2024,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2049,26 +2057,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2101,23 +2092,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2294,13 +2268,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:D88"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="34.875" customWidth="1"/>
     <col min="2" max="2" width="73.875" customWidth="1"/>
@@ -2311,7 +2285,7 @@
     <col min="7" max="7" width="37.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2330,7 +2304,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2351,7 +2325,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>293</v>
       </c>
@@ -2366,7 +2340,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -2389,7 +2363,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
         <v>110</v>
       </c>
@@ -2410,7 +2384,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2425,7 +2399,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -2438,7 +2412,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>230</v>
       </c>
@@ -2459,7 +2433,7 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
         <v>231</v>
       </c>
@@ -2474,7 +2448,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -2489,7 +2463,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="15" customFormat="1">
       <c r="A11" s="23" t="s">
         <v>278</v>
       </c>
@@ -2506,7 +2480,7 @@
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="15" customFormat="1">
       <c r="A12" s="23" t="s">
         <v>279</v>
       </c>
@@ -2521,7 +2495,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
         <v>234</v>
       </c>
@@ -2540,7 +2514,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
         <v>236</v>
       </c>
@@ -2557,7 +2531,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
@@ -2578,7 +2552,7 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
         <v>282</v>
       </c>
@@ -2595,7 +2569,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
         <v>101</v>
       </c>
@@ -2616,7 +2590,7 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
         <v>302</v>
       </c>
@@ -2631,7 +2605,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
@@ -2652,7 +2626,7 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
@@ -2673,7 +2647,7 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
@@ -2694,7 +2668,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>244</v>
       </c>
@@ -2713,7 +2687,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
@@ -2732,7 +2706,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
         <v>44</v>
       </c>
@@ -2753,7 +2727,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
         <v>47</v>
       </c>
@@ -2770,7 +2744,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2779,7 +2753,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
@@ -2798,7 +2772,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
@@ -2817,7 +2791,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
         <v>303</v>
       </c>
@@ -2836,7 +2810,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
         <v>63</v>
       </c>
@@ -2855,7 +2829,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
         <v>64</v>
       </c>
@@ -2874,7 +2848,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>65</v>
       </c>
@@ -2891,7 +2865,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>66</v>
       </c>
@@ -2910,7 +2884,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>67</v>
       </c>
@@ -2929,7 +2903,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>203</v>
       </c>
@@ -2948,7 +2922,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>204</v>
       </c>
@@ -2965,7 +2939,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>71</v>
       </c>
@@ -2984,7 +2958,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
         <v>197</v>
       </c>
@@ -3003,7 +2977,7 @@
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7">
       <c r="A39" s="10" t="s">
         <v>83</v>
       </c>
@@ -3024,7 +2998,7 @@
       </c>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>88</v>
       </c>
@@ -3043,7 +3017,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
         <v>96</v>
       </c>
@@ -3064,7 +3038,7 @@
       </c>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
         <v>109</v>
       </c>
@@ -3083,7 +3057,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
         <v>207</v>
       </c>
@@ -3100,7 +3074,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
         <v>225</v>
       </c>
@@ -3119,7 +3093,7 @@
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
         <v>224</v>
       </c>
@@ -3136,7 +3110,7 @@
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
         <v>256</v>
       </c>
@@ -3155,7 +3129,7 @@
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>260</v>
       </c>
@@ -3172,7 +3146,7 @@
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>297</v>
       </c>
@@ -3189,7 +3163,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
     </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" ht="12.75" customHeight="1">
       <c r="A49" s="10" t="s">
         <v>112</v>
       </c>
@@ -3208,7 +3182,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7" ht="15" customHeight="1">
       <c r="A50" s="11" t="s">
         <v>265</v>
       </c>
@@ -3225,7 +3199,7 @@
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7">
       <c r="A51" s="11" t="s">
         <v>115</v>
       </c>
@@ -3244,7 +3218,7 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7">
       <c r="A52" s="10" t="s">
         <v>114</v>
       </c>
@@ -3263,7 +3237,7 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7">
       <c r="A53" s="10" t="s">
         <v>253</v>
       </c>
@@ -3280,7 +3254,7 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
         <v>254</v>
       </c>
@@ -3297,7 +3271,7 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7">
       <c r="A55" s="10" t="s">
         <v>268</v>
       </c>
@@ -3314,7 +3288,7 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
         <v>287</v>
       </c>
@@ -3335,7 +3309,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7" s="15" customFormat="1">
       <c r="A57" s="23" t="s">
         <v>288</v>
       </c>
@@ -3352,7 +3326,7 @@
       <c r="F57" s="23"/>
       <c r="G57" s="23"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
         <v>134</v>
       </c>
@@ -3369,7 +3343,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7">
       <c r="A59" s="10" t="s">
         <v>137</v>
       </c>
@@ -3386,7 +3360,7 @@
       <c r="F59" s="9"/>
       <c r="G59" s="10"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:7">
       <c r="A60" s="10" t="s">
         <v>130</v>
       </c>
@@ -3405,7 +3379,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:7">
       <c r="A61" s="10" t="s">
         <v>127</v>
       </c>
@@ -3422,7 +3396,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7">
       <c r="A62" s="10"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
@@ -3431,7 +3405,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:7">
       <c r="A63" s="10" t="s">
         <v>142</v>
       </c>
@@ -3450,7 +3424,7 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:7">
       <c r="A64" s="11" t="s">
         <v>143</v>
       </c>
@@ -3469,7 +3443,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7">
       <c r="A65" s="11"/>
       <c r="B65" s="22"/>
       <c r="C65" s="10"/>
@@ -3478,7 +3452,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:7">
       <c r="A66" s="11" t="s">
         <v>309</v>
       </c>
@@ -3493,7 +3467,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:7">
       <c r="A67" s="43"/>
       <c r="B67" s="4"/>
       <c r="C67" s="43"/>
@@ -3502,7 +3476,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:7">
       <c r="A68" s="43"/>
       <c r="B68" s="4"/>
       <c r="C68" s="43"/>
@@ -3511,7 +3485,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:7" ht="44.25" customHeight="1">
       <c r="A69" s="47" t="s">
         <v>321</v>
       </c>
@@ -3522,7 +3496,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:7" ht="20.25" customHeight="1">
       <c r="A70" s="12" t="s">
         <v>322</v>
       </c>
@@ -3541,7 +3515,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:7" ht="20.25" customHeight="1">
       <c r="A71" s="12" t="s">
         <v>324</v>
       </c>
@@ -3558,7 +3532,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:7" ht="20.25" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>337</v>
       </c>
@@ -3572,7 +3546,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
     </row>
-    <row r="73" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7" ht="20.25" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>339</v>
       </c>
@@ -3586,7 +3560,7 @@
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
     </row>
-    <row r="74" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:7" ht="20.25" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>342</v>
       </c>
@@ -3600,7 +3574,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:7" ht="20.25" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>344</v>
       </c>
@@ -3614,7 +3588,7 @@
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
     </row>
-    <row r="76" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:7" ht="20.25" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>347</v>
       </c>
@@ -3628,7 +3602,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
     </row>
-    <row r="77" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:7" ht="20.25" customHeight="1">
       <c r="A77" s="4" t="s">
         <v>349</v>
       </c>
@@ -3642,7 +3616,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
     </row>
-    <row r="78" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:7" ht="20.25" customHeight="1">
       <c r="A78" s="43" t="s">
         <v>355</v>
       </c>
@@ -3659,7 +3633,7 @@
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
     </row>
-    <row r="79" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:7" ht="20.25" customHeight="1">
       <c r="A79" s="43" t="s">
         <v>350</v>
       </c>
@@ -3676,7 +3650,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
     </row>
-    <row r="80" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:7" ht="20.25" customHeight="1">
       <c r="A80" s="43" t="s">
         <v>357</v>
       </c>
@@ -3693,7 +3667,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
     </row>
-    <row r="81" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:7" ht="20.25" customHeight="1">
       <c r="A81" s="43" t="s">
         <v>358</v>
       </c>
@@ -3710,7 +3684,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
     </row>
-    <row r="82" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:7" ht="20.25" customHeight="1">
       <c r="A82" s="43" t="s">
         <v>365</v>
       </c>
@@ -3723,7 +3697,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:7" ht="20.25" customHeight="1">
       <c r="A83" s="43" t="s">
         <v>370</v>
       </c>
@@ -3740,7 +3714,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:7" ht="20.25" customHeight="1">
       <c r="A84" s="43" t="s">
         <v>375</v>
       </c>
@@ -3755,7 +3729,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
     </row>
-    <row r="85" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:7" ht="20.25" customHeight="1">
       <c r="A85" s="43" t="s">
         <v>378</v>
       </c>
@@ -3772,7 +3746,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
     </row>
-    <row r="86" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:7" ht="20.25" customHeight="1">
       <c r="A86" s="43" t="s">
         <v>382</v>
       </c>
@@ -3789,7 +3763,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
     </row>
-    <row r="87" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:7" ht="20.25" customHeight="1">
       <c r="A87" s="43" t="s">
         <v>386</v>
       </c>
@@ -3806,13 +3780,21 @@
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
     </row>
-    <row r="88" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:7" ht="40.5" customHeight="1">
       <c r="A88" s="46" t="s">
         <v>23</v>
       </c>
       <c r="B88" s="46"/>
       <c r="C88" s="46"/>
       <c r="D88" s="46"/>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>390</v>
+      </c>
+      <c r="B90" t="s">
+        <v>391</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3833,13 +3815,13 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="117.875" customWidth="1"/>
     <col min="2" max="2" width="37.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>162</v>
       </c>
@@ -3847,7 +3829,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -3855,7 +3837,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -3863,7 +3845,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>159</v>
       </c>
@@ -3871,7 +3853,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -3879,7 +3861,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -3887,7 +3869,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -3895,7 +3877,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -3903,7 +3885,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -3911,12 +3893,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -3924,7 +3906,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -3932,7 +3914,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -3940,7 +3922,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>150</v>
       </c>
@@ -3948,7 +3930,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -3956,7 +3938,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -3964,7 +3946,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>147</v>
       </c>
@@ -3972,7 +3954,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3994,13 +3976,13 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="75.875" customWidth="1"/>
     <col min="2" max="2" width="51.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="19" t="s">
         <v>192</v>
       </c>
@@ -4008,7 +3990,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="20" t="s">
         <v>187</v>
       </c>
@@ -4016,12 +3998,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="20" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" s="20" t="s">
         <v>189</v>
       </c>
@@ -4029,42 +4011,42 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="20" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="16" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" s="20" t="s">
         <v>201</v>
       </c>
@@ -4072,12 +4054,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>217</v>
       </c>
@@ -4097,13 +4079,13 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:12" ht="33.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:12" ht="30.75" customHeight="1">
       <c r="B2" s="28" t="s">
         <v>315</v>
       </c>
@@ -4124,7 +4106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12" ht="29.25" customHeight="1">
       <c r="B3" s="31">
         <v>4</v>
       </c>
@@ -4143,7 +4125,7 @@
       <c r="K3" s="35"/>
       <c r="L3" s="36"/>
     </row>
-    <row r="4" spans="2:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12" ht="35.25" customHeight="1">
       <c r="B4" s="37"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
@@ -4158,7 +4140,7 @@
       <c r="K4" s="38"/>
       <c r="L4" s="39"/>
     </row>
-    <row r="5" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12" ht="36.75" customHeight="1">
       <c r="B5" s="40"/>
       <c r="C5" s="27">
         <v>2</v>
@@ -4175,7 +4157,7 @@
       <c r="K5" s="35"/>
       <c r="L5" s="36"/>
     </row>
-    <row r="6" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12" ht="42" customHeight="1">
       <c r="B6" s="37"/>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
@@ -4192,7 +4174,7 @@
       <c r="K6" s="38"/>
       <c r="L6" s="39"/>
     </row>
-    <row r="7" spans="2:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12" ht="32.25" customHeight="1">
       <c r="B7" s="31"/>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
@@ -4207,7 +4189,7 @@
       <c r="K7" s="27"/>
       <c r="L7" s="32"/>
     </row>
-    <row r="8" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12" ht="41.25" customHeight="1">
       <c r="B8" s="37"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -4224,7 +4206,7 @@
       </c>
       <c r="L8" s="39"/>
     </row>
-    <row r="9" spans="2:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12" ht="38.25" customHeight="1">
       <c r="B9" s="40"/>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
@@ -4241,7 +4223,7 @@
       <c r="K9" s="35"/>
       <c r="L9" s="36"/>
     </row>
-    <row r="10" spans="2:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12" ht="39.75" customHeight="1">
       <c r="B10" s="37"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -4256,7 +4238,7 @@
       <c r="K10" s="38"/>
       <c r="L10" s="39"/>
     </row>
-    <row r="11" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12" ht="41.25" customHeight="1">
       <c r="B11" s="31">
         <v>7</v>
       </c>
@@ -4275,7 +4257,7 @@
       </c>
       <c r="L11" s="36"/>
     </row>
-    <row r="12" spans="2:12" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="44.25" customHeight="1" thickBot="1">
       <c r="B12" s="33">
         <v>10</v>
       </c>

</xml_diff>